<commit_message>
Updated Absolute best lap
now works more frequently and with less bugs (changed the less than to a greater than)
</commit_message>
<xml_diff>
--- a/Leaderboard.xlsx
+++ b/Leaderboard.xlsx
@@ -453,30 +453,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Noah</t>
+          <t>vfdvfd</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13.5</v>
+        <v>17</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>dfvkjdfn</t>
+          <t>ekjnerk</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>1200</t>
         </is>
       </c>
     </row>

</xml_diff>